<commit_message>
clean up preprocessing code and update qc logbook
</commit_message>
<xml_diff>
--- a/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
+++ b/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Nexus365\Project\pirate_fmri\Analysis\data\fmri\qualitycheck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/sedm6713_ox_ac_uk/Documents/Project/pirate_fmri/Analysis/data/fmri/qualitycheck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4383E1DD-E2B3-4C80-983A-C71FAD05F277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="8_{A85720FE-180F-422D-9118-C1E01BA6038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D28FB416-F981-4395-8169-3C8A64F16AB3}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="11016" windowHeight="18816" xr2:uid="{81260E08-A32C-4A7A-8C54-F109A8A5CB5F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{81260E08-A32C-4A7A-8C54-F109A8A5CB5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>subid</t>
   </si>
@@ -146,10 +147,79 @@
     <t>1. blury image near the edge of the brain at prefrontal region, is that normal? This is still there after unwarping. Eg sub005, sub006, sub015, sub017, sub018 sub023 task1 run1</t>
   </si>
   <si>
-    <t>check the realigned and unwarped images, select a random timepoint to check signal loss in the brain</t>
-  </si>
-  <si>
-    <t>check the normalized image</t>
+    <t>reorientation</t>
+  </si>
+  <si>
+    <t>ac-pc axis</t>
+  </si>
+  <si>
+    <t>origin to ac</t>
+  </si>
+  <si>
+    <t>fieldmap and unwarp</t>
+  </si>
+  <si>
+    <t>a bit off on z axis</t>
+  </si>
+  <si>
+    <t>quite off on z axis, almost to the bottom of prefrontal cortex</t>
+  </si>
+  <si>
+    <t>a bit off on y, quite off on z, almost to the bottom of prefrontal cortex</t>
+  </si>
+  <si>
+    <t>could pitch back a bit (negative pitch)</t>
+  </si>
+  <si>
+    <t>yawed a bit too much</t>
+  </si>
+  <si>
+    <t>check the realigned and unwarped images at a random timepoint to check signal loss in the brain</t>
+  </si>
+  <si>
+    <t>coregistration</t>
+  </si>
+  <si>
+    <t>check if t1 is coregistered well with meanepi</t>
+  </si>
+  <si>
+    <t>normalization</t>
+  </si>
+  <si>
+    <t>head movement</t>
+  </si>
+  <si>
+    <t>check if the epis looks like the template after normalization</t>
+  </si>
+  <si>
+    <t>absolute max displacement from first frame value smaller than</t>
+  </si>
+  <si>
+    <t>absolute max framewise displacement value smaller than</t>
+  </si>
+  <si>
+    <t>2 in localizer task and 2 in maintask run3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> some small shifts in both all task runs</t>
+  </si>
+  <si>
+    <t>1 big shift in localizer task, 1 small shift in main task run3 1 in maintask run 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> some small sudden shifts in all task runs</t>
+  </si>
+  <si>
+    <t>no sudden shift (smal/big sudden shift: smaller/bigger than voxel size)</t>
+  </si>
+  <si>
+    <t>2 big shift in localizer</t>
+  </si>
+  <si>
+    <t>the head movement parameters are (slightly) different for pipeline with and without reorientation in the beginning, does it matter? If so, which is more reliable?</t>
+  </si>
+  <si>
+    <t>constructing nuisance regressors for sudden head movement</t>
   </si>
 </sst>
 </file>
@@ -191,10 +261,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -211,6 +287,76 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F842D1-9C4B-D6AB-9075-EB29DB64E3F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2381250" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,302 +656,988 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D90649C-05E8-4A62-B4BC-85F3ED8A4C4F}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.36328125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7265625" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="5" width="25.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="8" max="10" width="14.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="J33"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="1:10" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
+      <c r="E36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:2" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="E37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D36:E36"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6672D9-BB03-4F65-AF41-2C4C215570C6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change link to quanlity check log book
</commit_message>
<xml_diff>
--- a/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
+++ b/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/sedm6713_ox_ac_uk/Documents/Project/pirate_fmri/Analysis/data/fmri/qualitycheck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="8_{A85720FE-180F-422D-9118-C1E01BA6038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D28FB416-F981-4395-8169-3C8A64F16AB3}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{A85720FE-180F-422D-9118-C1E01BA6038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6592A3A6-F1EC-493A-A6D1-AF214CB2014B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{81260E08-A32C-4A7A-8C54-F109A8A5CB5F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{81260E08-A32C-4A7A-8C54-F109A8A5CB5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
   <si>
     <t>subid</t>
   </si>
@@ -219,25 +219,49 @@
     <t>the head movement parameters are (slightly) different for pipeline with and without reorientation in the beginning, does it matter? If so, which is more reliable?</t>
   </si>
   <si>
-    <t>constructing nuisance regressors for sudden head movement</t>
+    <t>1 small shift in main task run1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 in localizer task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>some in all runs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constructing nuisance regressors for sudden head movement: what count as sudden head movement (framewise displacement &gt; voxel size?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -353,10 +377,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -659,19 +679,22 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="5" width="25.54296875" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="10" width="14.90625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.73046875" customWidth="1"/>
+    <col min="4" max="5" width="25.53125" customWidth="1"/>
+    <col min="6" max="6" width="19.46484375" customWidth="1"/>
+    <col min="7" max="7" width="18.46484375" customWidth="1"/>
+    <col min="8" max="10" width="14.9296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -695,7 +718,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>37</v>
@@ -725,7 +748,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -753,11 +776,11 @@
       <c r="I3" s="1">
         <v>0.2</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -789,7 +812,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -821,7 +844,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -853,7 +876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -885,7 +908,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -913,11 +936,11 @@
       <c r="I8" s="1">
         <v>0.2</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -945,11 +968,11 @@
       <c r="I9" s="1">
         <v>0.2</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -977,11 +1000,11 @@
       <c r="I10" s="1">
         <v>0.2</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1009,11 +1032,11 @@
       <c r="I11" s="1">
         <v>0.2</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1041,11 +1064,11 @@
       <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1073,11 +1096,11 @@
       <c r="I13" s="1">
         <v>0.5</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1132,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1137,11 +1160,11 @@
       <c r="I15" s="1">
         <v>0.2</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1196,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1195,9 +1218,17 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1219,9 +1250,17 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1243,9 +1282,17 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1267,9 +1314,17 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1291,9 +1346,17 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1315,9 +1378,17 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H22" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1339,9 +1410,17 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1363,9 +1442,17 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1387,9 +1474,17 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1411,9 +1506,17 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1435,9 +1538,17 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1459,9 +1570,17 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1483,9 +1602,17 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1507,9 +1634,17 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1531,9 +1666,17 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1555,9 +1698,17 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H32" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1581,12 +1732,12 @@
       </c>
       <c r="J33"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="101" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1597,22 +1748,22 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:10" ht="92.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="1:10" ht="92.55" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D37:E37"/>
@@ -1635,8 +1786,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed bug in tsnr calculation
</commit_message>
<xml_diff>
--- a/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
+++ b/data/fmri/qualitycheck/QualityCheckLogBook.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,14 +10,15 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="320" documentId="8_{A85720FE-180F-422D-9118-C1E01BA6038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F5886D-2DC4-4ACA-A39D-3799D9921B79}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="headmotion" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="tsnr" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="62">
   <si>
     <t>subid</t>
   </si>
@@ -210,6 +211,21 @@
   <si>
     <t>percentage of outliers - framewise displacement (%)</t>
   </si>
+  <si>
+    <t>AAL_Occipital.nii</t>
+  </si>
+  <si>
+    <t>AAL_ParaHippocampus.nii</t>
+  </si>
+  <si>
+    <t>AAL_Prefrontal.nii</t>
+  </si>
+  <si>
+    <t>Anatomy_Hippocampus.nii</t>
+  </si>
+  <si>
+    <t>EC.nii</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -253,21 +269,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -286,7 +304,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -304,19 +322,19 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+            <a:ext xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F842D1-9C4B-D6AB-9075-EB29DB64E3F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="true" noChangeArrowheads="true"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip r:embed="rId1">
           <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+            <a:ext xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
@@ -336,7 +354,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -648,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D90649C-05E8-4A62-B4BC-85F3ED8A4C4F}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
@@ -659,13 +677,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" customWidth="true"/>
+    <col min="4" max="5" width="25.42578125" customWidth="true"/>
+    <col min="6" max="6" width="19.42578125" customWidth="true"/>
+    <col min="7" max="7" width="18.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.1" customHeight="1">
+    <row r="1" ht="29.1" customHeight="true">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -684,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="88.5" customHeight="1">
+    <row r="2" s="1" customFormat="true" ht="88.5" customHeight="true">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -705,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -728,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -751,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -774,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -797,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -820,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -843,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -866,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -889,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -912,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -935,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -958,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -981,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1027,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1050,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1073,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1119,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1142,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1188,7 +1206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1211,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1234,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1257,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1280,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1303,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1326,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1349,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1372,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1395,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" hidden="true">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1418,28 +1436,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35">
       <c r="A35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="101.1" customHeight="1">
+    <row r="36" ht="101.1" customHeight="true">
       <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="92.65" customHeight="1">
+    <row r="37" ht="92.65" customHeight="true">
       <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="92.65" customHeight="1"/>
-    <row r="39" spans="1:7" ht="92.65" customHeight="1"/>
-    <row r="40" spans="1:7" ht="92.65" customHeight="1"/>
-    <row r="41" spans="1:7" ht="92.65" customHeight="1"/>
-    <row r="42" spans="1:7" ht="92.65" customHeight="1"/>
+    <row r="38" ht="92.65" customHeight="true"/>
+    <row r="39" ht="92.65" customHeight="true"/>
+    <row r="40" ht="92.65" customHeight="true"/>
+    <row r="41" ht="92.65" customHeight="true"/>
+    <row r="42" ht="92.65" customHeight="true"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D37:E37"/>
@@ -1457,20 +1475,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="true"/>
+    <col min="2" max="2" width="42.140625" customWidth="true"/>
+    <col min="3" max="3" width="43.85546875" customWidth="true"/>
+    <col min="4" max="4" width="49.7109375" customWidth="true"/>
+    <col min="5" max="5" width="38.85546875" customWidth="true"/>
+    <col min="6" max="6" width="38.5703125" customWidth="true"/>
+    <col min="7" max="7" width="44.28515625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1493,7 +1511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1516,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1608,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1631,7 +1649,7 @@
         <v>6.1538461538461538E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1654,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1677,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1700,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1723,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>6.7796610169491523E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1815,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1838,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1861,7 +1879,7 @@
         <v>3.0769230769230769E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1884,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1930,7 +1948,7 @@
         <v>3.3898305084745762E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1953,7 +1971,7 @@
         <v>3.3898305084745762E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1976,7 +1994,7 @@
         <v>3.0769230769230769E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1999,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2091,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2114,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2160,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2183,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2206,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2229,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2252,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -2275,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2298,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2321,7 +2339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2344,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2367,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -2390,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2413,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2436,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -2459,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -2482,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -2528,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -2574,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -2597,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2620,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -2643,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -2666,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -2689,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -2712,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -2735,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -2758,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -2781,7 +2799,7 @@
         <v>2.1538461538461538E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>8.8135593220338981E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -2827,7 +2845,7 @@
         <v>4.7457627118644069E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2850,7 +2868,7 @@
         <v>2.3728813559322035E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -2873,7 +2891,7 @@
         <v>3.0508474576271188E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -2896,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -2919,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2942,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -2965,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -2988,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>1.8461538461538463E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -3034,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -3057,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3103,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -3126,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73">
       <c r="A73" t="s">
         <v>29</v>
       </c>
@@ -3149,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -3172,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -3195,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76">
       <c r="A76" t="s">
         <v>29</v>
       </c>
@@ -3218,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -3241,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -3264,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79">
       <c r="A79" t="s">
         <v>30</v>
       </c>
@@ -3287,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -3310,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -3333,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82">
       <c r="A82" t="s">
         <v>31</v>
       </c>
@@ -3356,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -3379,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -3402,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -3425,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -3448,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87">
       <c r="A87" t="s">
         <v>32</v>
       </c>
@@ -3471,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88">
       <c r="A88" t="s">
         <v>32</v>
       </c>
@@ -3494,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89">
       <c r="A89" t="s">
         <v>32</v>
       </c>
@@ -3517,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90">
       <c r="A90" t="s">
         <v>32</v>
       </c>
@@ -3540,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91">
       <c r="A91" t="s">
         <v>32</v>
       </c>
@@ -3563,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92">
       <c r="A92" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +3604,7 @@
         <v>3.0769230769230769E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93">
       <c r="A93" t="s">
         <v>33</v>
       </c>
@@ -3609,7 +3627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94">
       <c r="A94" t="s">
         <v>33</v>
       </c>
@@ -3632,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95">
       <c r="A95" t="s">
         <v>33</v>
       </c>
@@ -3655,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96">
       <c r="A96" t="s">
         <v>33</v>
       </c>
@@ -3678,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -3701,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98">
       <c r="A98" t="s">
         <v>34</v>
       </c>
@@ -3724,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -3747,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100">
       <c r="A100" t="s">
         <v>34</v>
       </c>
@@ -3770,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101">
       <c r="A101" t="s">
         <v>34</v>
       </c>
@@ -3793,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -3816,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103">
       <c r="A103" t="s">
         <v>35</v>
       </c>
@@ -3839,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104">
       <c r="A104" t="s">
         <v>35</v>
       </c>
@@ -3862,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -3885,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106">
       <c r="A106" t="s">
         <v>35</v>
       </c>
@@ -3908,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107">
       <c r="A107" t="s">
         <v>36</v>
       </c>
@@ -3931,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108">
       <c r="A108" t="s">
         <v>36</v>
       </c>
@@ -3954,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109">
       <c r="A109" t="s">
         <v>36</v>
       </c>
@@ -3977,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110">
       <c r="A110" t="s">
         <v>36</v>
       </c>
@@ -4000,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111">
       <c r="A111" t="s">
         <v>36</v>
       </c>
@@ -4023,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112">
       <c r="A112" t="s">
         <v>37</v>
       </c>
@@ -4046,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113">
       <c r="A113" t="s">
         <v>37</v>
       </c>
@@ -4069,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114">
       <c r="A114" t="s">
         <v>37</v>
       </c>
@@ -4092,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115">
       <c r="A115" t="s">
         <v>37</v>
       </c>
@@ -4115,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -4138,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117">
       <c r="A117" t="s">
         <v>38</v>
       </c>
@@ -4161,7 +4179,7 @@
         <v>3.0769230769230769E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119">
       <c r="A119" t="s">
         <v>38</v>
       </c>
@@ -4207,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120">
       <c r="A120" t="s">
         <v>38</v>
       </c>
@@ -4230,7 +4248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121">
       <c r="A121" t="s">
         <v>38</v>
       </c>
@@ -4253,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -4276,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123">
       <c r="A123" t="s">
         <v>39</v>
       </c>
@@ -4299,7 +4317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124">
       <c r="A124" t="s">
         <v>39</v>
       </c>
@@ -4322,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125">
       <c r="A125" t="s">
         <v>39</v>
       </c>
@@ -4345,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126">
       <c r="A126" t="s">
         <v>39</v>
       </c>
@@ -4368,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127">
       <c r="A127" t="s">
         <v>40</v>
       </c>
@@ -4391,7 +4409,7 @@
         <v>6.1538461538461538E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128">
       <c r="A128" t="s">
         <v>40</v>
       </c>
@@ -4414,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129">
       <c r="A129" t="s">
         <v>40</v>
       </c>
@@ -4437,7 +4455,7 @@
         <v>1.3559322033898305E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130">
       <c r="A130" t="s">
         <v>40</v>
       </c>
@@ -4460,7 +4478,7 @@
         <v>3.3898305084745762E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131">
       <c r="A131" t="s">
         <v>40</v>
       </c>
@@ -4483,7 +4501,7 @@
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132">
       <c r="A132" t="s">
         <v>41</v>
       </c>
@@ -4506,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -4529,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134">
       <c r="A134" t="s">
         <v>41</v>
       </c>
@@ -4552,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135">
       <c r="A135" t="s">
         <v>41</v>
       </c>
@@ -4575,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136">
       <c r="A136" t="s">
         <v>41</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -4621,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138">
       <c r="A138" t="s">
         <v>42</v>
       </c>
@@ -4644,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139">
       <c r="A139" t="s">
         <v>42</v>
       </c>
@@ -4667,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -4690,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -4713,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142">
       <c r="A142" t="s">
         <v>43</v>
       </c>
@@ -4736,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143">
       <c r="A143" t="s">
         <v>43</v>
       </c>
@@ -4759,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144">
       <c r="A144" t="s">
         <v>43</v>
       </c>
@@ -4782,7 +4800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145">
       <c r="A145" t="s">
         <v>43</v>
       </c>
@@ -4805,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146">
       <c r="A146" t="s">
         <v>43</v>
       </c>
@@ -4828,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147">
       <c r="A147" t="s">
         <v>45</v>
       </c>
@@ -4851,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148">
       <c r="A148" t="s">
         <v>45</v>
       </c>
@@ -4874,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149">
       <c r="A149" t="s">
         <v>45</v>
       </c>
@@ -4897,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150">
       <c r="A150" t="s">
         <v>45</v>
       </c>
@@ -4920,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151">
       <c r="A151" t="s">
         <v>45</v>
       </c>
@@ -4943,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152">
       <c r="A152" t="s">
         <v>46</v>
       </c>
@@ -4966,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153">
       <c r="A153" t="s">
         <v>46</v>
       </c>
@@ -4989,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154">
       <c r="A154" t="s">
         <v>46</v>
       </c>
@@ -5012,7 +5030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155">
       <c r="A155" t="s">
         <v>46</v>
       </c>
@@ -5052,4 +5070,2662 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E156"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.82421875" customWidth="true"/>
+    <col min="2" max="2" width="22.37890625" customWidth="true"/>
+    <col min="3" max="3" width="15.93359375" customWidth="true"/>
+    <col min="4" max="4" width="22.93359375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>86.331033531116319</v>
+      </c>
+      <c r="B2" s="0">
+        <v>39.511796733212343</v>
+      </c>
+      <c r="C2" s="0">
+        <v>68.79081967213115</v>
+      </c>
+      <c r="D2" s="0">
+        <v>25.192926045016076</v>
+      </c>
+      <c r="E2" s="0">
+        <v>16.992592592592594</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>78.023733958879532</v>
+      </c>
+      <c r="B3" s="0">
+        <v>34.946460980036299</v>
+      </c>
+      <c r="C3" s="0">
+        <v>57.067468123861566</v>
+      </c>
+      <c r="D3" s="0">
+        <v>22.630225080385852</v>
+      </c>
+      <c r="E3" s="0">
+        <v>15.459259259259259</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>82.370360149027178</v>
+      </c>
+      <c r="B4" s="0">
+        <v>37.224137931034484</v>
+      </c>
+      <c r="C4" s="0">
+        <v>67.344335154826965</v>
+      </c>
+      <c r="D4" s="0">
+        <v>23.729903536977492</v>
+      </c>
+      <c r="E4" s="0">
+        <v>16.199999999999999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>81.729819235545747</v>
+      </c>
+      <c r="B5" s="0">
+        <v>35.382032667876587</v>
+      </c>
+      <c r="C5" s="0">
+        <v>58.22550091074681</v>
+      </c>
+      <c r="D5" s="0">
+        <v>23.405144694533764</v>
+      </c>
+      <c r="E5" s="0">
+        <v>15.496296296296297</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>72.854008555264244</v>
+      </c>
+      <c r="B6" s="0">
+        <v>31.804900181488204</v>
+      </c>
+      <c r="C6" s="0">
+        <v>53.826593806921679</v>
+      </c>
+      <c r="D6" s="0">
+        <v>20.135048231511256</v>
+      </c>
+      <c r="E6" s="0">
+        <v>13.459259259259259</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>61.438940251138405</v>
+      </c>
+      <c r="B7" s="0">
+        <v>39.012704174228674</v>
+      </c>
+      <c r="C7" s="0">
+        <v>55.211876138433517</v>
+      </c>
+      <c r="D7" s="0">
+        <v>28.2540192926045</v>
+      </c>
+      <c r="E7" s="0">
+        <v>23.118518518518517</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>58.377397543811234</v>
+      </c>
+      <c r="B8" s="0">
+        <v>37.107985480943739</v>
+      </c>
+      <c r="C8" s="0">
+        <v>59.712786885245905</v>
+      </c>
+      <c r="D8" s="0">
+        <v>28.60450160771704</v>
+      </c>
+      <c r="E8" s="0">
+        <v>22.185185185185187</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>57.193735338760867</v>
+      </c>
+      <c r="B9" s="0">
+        <v>38.249546279491831</v>
+      </c>
+      <c r="C9" s="0">
+        <v>51.290856102003644</v>
+      </c>
+      <c r="D9" s="0">
+        <v>27.466237942122188</v>
+      </c>
+      <c r="E9" s="0">
+        <v>23.42962962962963</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>67.661653097833593</v>
+      </c>
+      <c r="B10" s="0">
+        <v>40.941923774954631</v>
+      </c>
+      <c r="C10" s="0">
+        <v>57.287285974499092</v>
+      </c>
+      <c r="D10" s="0">
+        <v>31.286173633440516</v>
+      </c>
+      <c r="E10" s="0">
+        <v>24.903703703703705</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>59.608803642886713</v>
+      </c>
+      <c r="B11" s="0">
+        <v>40.55263157894737</v>
+      </c>
+      <c r="C11" s="0">
+        <v>55.379453551912569</v>
+      </c>
+      <c r="D11" s="0">
+        <v>28.906752411575564</v>
+      </c>
+      <c r="E11" s="0">
+        <v>23.600000000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>67.115358079205194</v>
+      </c>
+      <c r="B12" s="0">
+        <v>39.930127041742288</v>
+      </c>
+      <c r="C12" s="0">
+        <v>67.924954462659386</v>
+      </c>
+      <c r="D12" s="0">
+        <v>31.627009646302252</v>
+      </c>
+      <c r="E12" s="0">
+        <v>19.785185185185185</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>68.626604112046365</v>
+      </c>
+      <c r="B13" s="0">
+        <v>35.649727767695097</v>
+      </c>
+      <c r="C13" s="0">
+        <v>64.922622950819672</v>
+      </c>
+      <c r="D13" s="0">
+        <v>28.118971061093248</v>
+      </c>
+      <c r="E13" s="0">
+        <v>17.548148148148147</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>67.908513867807372</v>
+      </c>
+      <c r="B14" s="0">
+        <v>37.26678765880218</v>
+      </c>
+      <c r="C14" s="0">
+        <v>56.74462659380692</v>
+      </c>
+      <c r="D14" s="0">
+        <v>27.909967845659164</v>
+      </c>
+      <c r="E14" s="0">
+        <v>18.05185185185185</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>76.861321926314332</v>
+      </c>
+      <c r="B15" s="0">
+        <v>40.908348457350272</v>
+      </c>
+      <c r="C15" s="0">
+        <v>68.464845173041894</v>
+      </c>
+      <c r="D15" s="0">
+        <v>31.39549839228296</v>
+      </c>
+      <c r="E15" s="0">
+        <v>20.325925925925926</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>75.102249206568231</v>
+      </c>
+      <c r="B16" s="0">
+        <v>37.280399274047184</v>
+      </c>
+      <c r="C16" s="0">
+        <v>61.067978142076505</v>
+      </c>
+      <c r="D16" s="0">
+        <v>28.192926045016076</v>
+      </c>
+      <c r="E16" s="0">
+        <v>18.237037037037037</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>56.455636815233888</v>
+      </c>
+      <c r="B17" s="0">
+        <v>26.125226860254084</v>
+      </c>
+      <c r="C17" s="0">
+        <v>44.399198542805102</v>
+      </c>
+      <c r="D17" s="0">
+        <v>17.922829581993568</v>
+      </c>
+      <c r="E17" s="0">
+        <v>11.185185185185185</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>72.397819787498278</v>
+      </c>
+      <c r="B18" s="0">
+        <v>37.218693284936478</v>
+      </c>
+      <c r="C18" s="0">
+        <v>70.476357012750455</v>
+      </c>
+      <c r="D18" s="0">
+        <v>25.720257234726688</v>
+      </c>
+      <c r="E18" s="0">
+        <v>17.800000000000001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>70.128880916241201</v>
+      </c>
+      <c r="B19" s="0">
+        <v>36.138838475499092</v>
+      </c>
+      <c r="C19" s="0">
+        <v>69.213624772313295</v>
+      </c>
+      <c r="D19" s="0">
+        <v>25.289389067524116</v>
+      </c>
+      <c r="E19" s="0">
+        <v>17.340740740740742</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>66.930591969090656</v>
+      </c>
+      <c r="B20" s="0">
+        <v>35.360254083484577</v>
+      </c>
+      <c r="C20" s="0">
+        <v>60.852531876138436</v>
+      </c>
+      <c r="D20" s="0">
+        <v>24.057877813504824</v>
+      </c>
+      <c r="E20" s="0">
+        <v>15.955555555555556</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>58.96370912101559</v>
+      </c>
+      <c r="B21" s="0">
+        <v>27.591651542649728</v>
+      </c>
+      <c r="C21" s="0">
+        <v>48.171657559198543</v>
+      </c>
+      <c r="D21" s="0">
+        <v>19.167202572347268</v>
+      </c>
+      <c r="E21" s="0">
+        <v>11.97037037037037</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>51.055747205740303</v>
+      </c>
+      <c r="B22" s="0">
+        <v>25.944646098003631</v>
+      </c>
+      <c r="C22" s="0">
+        <v>45.798761384335158</v>
+      </c>
+      <c r="D22" s="0">
+        <v>14.440514469453376</v>
+      </c>
+      <c r="E22" s="0">
+        <v>11.496296296296297</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>52.878570442941907</v>
+      </c>
+      <c r="B23" s="0">
+        <v>29.641560798548095</v>
+      </c>
+      <c r="C23" s="0">
+        <v>50.939453551912571</v>
+      </c>
+      <c r="D23" s="0">
+        <v>16.520900321543408</v>
+      </c>
+      <c r="E23" s="0">
+        <v>13.562962962962963</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>61.611701393680143</v>
+      </c>
+      <c r="B24" s="0">
+        <v>30.882032667876587</v>
+      </c>
+      <c r="C24" s="0">
+        <v>54.375883424408016</v>
+      </c>
+      <c r="D24" s="0">
+        <v>16.881028938906752</v>
+      </c>
+      <c r="E24" s="0">
+        <v>13.800000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>53.422519663308954</v>
+      </c>
+      <c r="B25" s="0">
+        <v>26.46551724137931</v>
+      </c>
+      <c r="C25" s="0">
+        <v>48.929471766848813</v>
+      </c>
+      <c r="D25" s="0">
+        <v>15.92282958199357</v>
+      </c>
+      <c r="E25" s="0">
+        <v>11.407407407407407</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>52.10652683869187</v>
+      </c>
+      <c r="B26" s="0">
+        <v>27.376588021778584</v>
+      </c>
+      <c r="C26" s="0">
+        <v>50.494280510018214</v>
+      </c>
+      <c r="D26" s="0">
+        <v>16.070739549839228</v>
+      </c>
+      <c r="E26" s="0">
+        <v>12.355555555555556</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>74.444183800193187</v>
+      </c>
+      <c r="B27" s="0">
+        <v>47.009981851179674</v>
+      </c>
+      <c r="C27" s="0">
+        <v>75.497923497267763</v>
+      </c>
+      <c r="D27" s="0">
+        <v>41.90032154340836</v>
+      </c>
+      <c r="E27" s="0">
+        <v>29.703703703703702</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>64.579136194287287</v>
+      </c>
+      <c r="B28" s="0">
+        <v>39.17695099818512</v>
+      </c>
+      <c r="C28" s="0">
+        <v>60.277231329690345</v>
+      </c>
+      <c r="D28" s="0">
+        <v>34.961414790996784</v>
+      </c>
+      <c r="E28" s="0">
+        <v>25.31111111111111</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>80.598868497309226</v>
+      </c>
+      <c r="B29" s="0">
+        <v>48.878402903811249</v>
+      </c>
+      <c r="C29" s="0">
+        <v>83.969617486338791</v>
+      </c>
+      <c r="D29" s="0">
+        <v>43.739549839228296</v>
+      </c>
+      <c r="E29" s="0">
+        <v>30.866666666666667</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>71.714916517179518</v>
+      </c>
+      <c r="B30" s="0">
+        <v>47.787658802177859</v>
+      </c>
+      <c r="C30" s="0">
+        <v>77.859599271402544</v>
+      </c>
+      <c r="D30" s="0">
+        <v>43.514469453376208</v>
+      </c>
+      <c r="E30" s="0">
+        <v>31.185185185185187</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>75.919138954049956</v>
+      </c>
+      <c r="B31" s="0">
+        <v>48.641560798548092</v>
+      </c>
+      <c r="C31" s="0">
+        <v>82.917595628415299</v>
+      </c>
+      <c r="D31" s="0">
+        <v>44.60128617363344</v>
+      </c>
+      <c r="E31" s="0">
+        <v>31.881481481481483</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>65.837036014902722</v>
+      </c>
+      <c r="B32" s="0">
+        <v>35.808529945553538</v>
+      </c>
+      <c r="C32" s="0">
+        <v>61.43978142076503</v>
+      </c>
+      <c r="D32" s="0">
+        <v>21.720257234726688</v>
+      </c>
+      <c r="E32" s="0">
+        <v>17.777777777777779</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>61.929626052159513</v>
+      </c>
+      <c r="B33" s="0">
+        <v>29.617967332123413</v>
+      </c>
+      <c r="C33" s="0">
+        <v>49.724225865209469</v>
+      </c>
+      <c r="D33" s="0">
+        <v>14.845659163987138</v>
+      </c>
+      <c r="E33" s="0">
+        <v>11.651851851851852</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>63.871119083758799</v>
+      </c>
+      <c r="B34" s="0">
+        <v>36.403811252268603</v>
+      </c>
+      <c r="C34" s="0">
+        <v>68.707249544626592</v>
+      </c>
+      <c r="D34" s="0">
+        <v>22.2508038585209</v>
+      </c>
+      <c r="E34" s="0">
+        <v>17.896296296296295</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>62.866151510970056</v>
+      </c>
+      <c r="B35" s="0">
+        <v>37.03448275862069</v>
+      </c>
+      <c r="C35" s="0">
+        <v>60.812167577413476</v>
+      </c>
+      <c r="D35" s="0">
+        <v>21.122186495176848</v>
+      </c>
+      <c r="E35" s="0">
+        <v>17.733333333333334</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>66.819373533876089</v>
+      </c>
+      <c r="B36" s="0">
+        <v>32.299455535390202</v>
+      </c>
+      <c r="C36" s="0">
+        <v>56.720218579234974</v>
+      </c>
+      <c r="D36" s="0">
+        <v>18.662379421221864</v>
+      </c>
+      <c r="E36" s="0">
+        <v>15.37037037037037</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>67.503656685525044</v>
+      </c>
+      <c r="B37" s="0">
+        <v>39.560798548094375</v>
+      </c>
+      <c r="C37" s="0">
+        <v>67.898069216757747</v>
+      </c>
+      <c r="D37" s="0">
+        <v>27.909967845659164</v>
+      </c>
+      <c r="E37" s="0">
+        <v>18.422222222222221</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>62.324548088864354</v>
+      </c>
+      <c r="B38" s="0">
+        <v>40.522686025408348</v>
+      </c>
+      <c r="C38" s="0">
+        <v>72.044808743169398</v>
+      </c>
+      <c r="D38" s="0">
+        <v>28.112540192926044</v>
+      </c>
+      <c r="E38" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>59.801573064716436</v>
+      </c>
+      <c r="B39" s="0">
+        <v>32.370235934664244</v>
+      </c>
+      <c r="C39" s="0">
+        <v>58.131220400728594</v>
+      </c>
+      <c r="D39" s="0">
+        <v>21.932475884244372</v>
+      </c>
+      <c r="E39" s="0">
+        <v>14.637037037037038</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>53.768317924658483</v>
+      </c>
+      <c r="B40" s="0">
+        <v>32.453720508166967</v>
+      </c>
+      <c r="C40" s="0">
+        <v>57.050054644808746</v>
+      </c>
+      <c r="D40" s="0">
+        <v>23.077170418006432</v>
+      </c>
+      <c r="E40" s="0">
+        <v>15.333333333333334</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>58.24934455636815</v>
+      </c>
+      <c r="B41" s="0">
+        <v>37.470054446460978</v>
+      </c>
+      <c r="C41" s="0">
+        <v>64.985209471766851</v>
+      </c>
+      <c r="D41" s="0">
+        <v>27.392282958199356</v>
+      </c>
+      <c r="E41" s="0">
+        <v>18.377777777777776</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>94.783220643024706</v>
+      </c>
+      <c r="B42" s="0">
+        <v>40.929219600725951</v>
+      </c>
+      <c r="C42" s="0">
+        <v>79.022149362477236</v>
+      </c>
+      <c r="D42" s="0">
+        <v>31.440514469453376</v>
+      </c>
+      <c r="E42" s="0">
+        <v>20.555555555555557</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>82.835242169173455</v>
+      </c>
+      <c r="B43" s="0">
+        <v>35.575317604355718</v>
+      </c>
+      <c r="C43" s="0">
+        <v>66.087650273224043</v>
+      </c>
+      <c r="D43" s="0">
+        <v>26.5016077170418</v>
+      </c>
+      <c r="E43" s="0">
+        <v>17.103703703703705</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>88.57044294190699</v>
+      </c>
+      <c r="B44" s="0">
+        <v>38.729582577132483</v>
+      </c>
+      <c r="C44" s="0">
+        <v>73.692313296903464</v>
+      </c>
+      <c r="D44" s="0">
+        <v>28.090032154340836</v>
+      </c>
+      <c r="E44" s="0">
+        <v>18.303703703703704</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>92.900786532358211</v>
+      </c>
+      <c r="B45" s="0">
+        <v>42.421960072595283</v>
+      </c>
+      <c r="C45" s="0">
+        <v>81.093989071038251</v>
+      </c>
+      <c r="D45" s="0">
+        <v>32.434083601286176</v>
+      </c>
+      <c r="E45" s="0">
+        <v>20.777777777777779</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>90.11756588933352</v>
+      </c>
+      <c r="B46" s="0">
+        <v>40.385662431941924</v>
+      </c>
+      <c r="C46" s="0">
+        <v>79.501639344262301</v>
+      </c>
+      <c r="D46" s="0">
+        <v>31.540192926045016</v>
+      </c>
+      <c r="E46" s="0">
+        <v>19.896296296296295</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>51.231130122809439</v>
+      </c>
+      <c r="B47" s="0">
+        <v>25.7513611615245</v>
+      </c>
+      <c r="C47" s="0">
+        <v>44.126338797814206</v>
+      </c>
+      <c r="D47" s="0">
+        <v>15.430868167202572</v>
+      </c>
+      <c r="E47" s="0">
+        <v>14.133333333333333</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>55.28287567269215</v>
+      </c>
+      <c r="B48" s="0">
+        <v>27.079854809437386</v>
+      </c>
+      <c r="C48" s="0">
+        <v>47.703825136612025</v>
+      </c>
+      <c r="D48" s="0">
+        <v>18</v>
+      </c>
+      <c r="E48" s="0">
+        <v>14.65925925925926</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>50.93266179108597</v>
+      </c>
+      <c r="B49" s="0">
+        <v>26.41923774954628</v>
+      </c>
+      <c r="C49" s="0">
+        <v>48.272276867030968</v>
+      </c>
+      <c r="D49" s="0">
+        <v>17.916398713826368</v>
+      </c>
+      <c r="E49" s="0">
+        <v>14.385185185185184</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>68.499379053401412</v>
+      </c>
+      <c r="B50" s="0">
+        <v>38.21415607985481</v>
+      </c>
+      <c r="C50" s="0">
+        <v>64.575737704918026</v>
+      </c>
+      <c r="D50" s="0">
+        <v>23.694533762057876</v>
+      </c>
+      <c r="E50" s="0">
+        <v>21.474074074074075</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>67.01159100317372</v>
+      </c>
+      <c r="B51" s="0">
+        <v>33.87295825771325</v>
+      </c>
+      <c r="C51" s="0">
+        <v>51.502367941712201</v>
+      </c>
+      <c r="D51" s="0">
+        <v>20.022508038585208</v>
+      </c>
+      <c r="E51" s="0">
+        <v>17.637037037037036</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>82.152200910721675</v>
+      </c>
+      <c r="B52" s="0">
+        <v>35.914700544464608</v>
+      </c>
+      <c r="C52" s="0">
+        <v>64.361967213114752</v>
+      </c>
+      <c r="D52" s="0">
+        <v>18.95176848874598</v>
+      </c>
+      <c r="E52" s="0">
+        <v>15.874074074074073</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>65.110252518283431</v>
+      </c>
+      <c r="B53" s="0">
+        <v>30.141560798548095</v>
+      </c>
+      <c r="C53" s="0">
+        <v>57.304043715846994</v>
+      </c>
+      <c r="D53" s="0">
+        <v>16.016077170418008</v>
+      </c>
+      <c r="E53" s="0">
+        <v>13.992592592592592</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>70.710776873188905</v>
+      </c>
+      <c r="B54" s="0">
+        <v>33.381125226860256</v>
+      </c>
+      <c r="C54" s="0">
+        <v>58.382805100182146</v>
+      </c>
+      <c r="D54" s="0">
+        <v>18.45016077170418</v>
+      </c>
+      <c r="E54" s="0">
+        <v>15.437037037037037</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>62.965916931143923</v>
+      </c>
+      <c r="B55" s="0">
+        <v>28.911070780399275</v>
+      </c>
+      <c r="C55" s="0">
+        <v>56.77253187613843</v>
+      </c>
+      <c r="D55" s="0">
+        <v>15.72347266881029</v>
+      </c>
+      <c r="E55" s="0">
+        <v>12.940740740740742</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>71.572236787636257</v>
+      </c>
+      <c r="B56" s="0">
+        <v>31.404718693284938</v>
+      </c>
+      <c r="C56" s="0">
+        <v>59.035774134790529</v>
+      </c>
+      <c r="D56" s="0">
+        <v>15.655948553054662</v>
+      </c>
+      <c r="E56" s="0">
+        <v>13.540740740740741</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>40.666896646888368</v>
+      </c>
+      <c r="B57" s="0">
+        <v>31.407441016333937</v>
+      </c>
+      <c r="C57" s="0">
+        <v>44.587759562841534</v>
+      </c>
+      <c r="D57" s="0">
+        <v>18.173633440514468</v>
+      </c>
+      <c r="E57" s="0">
+        <v>13.407407407407407</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>29.032427211259833</v>
+      </c>
+      <c r="B58" s="0">
+        <v>20.999092558983666</v>
+      </c>
+      <c r="C58" s="0">
+        <v>30.781420765027324</v>
+      </c>
+      <c r="D58" s="0">
+        <v>12.192926045016078</v>
+      </c>
+      <c r="E58" s="0">
+        <v>9.6518518518518519</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>33.426521319166554</v>
+      </c>
+      <c r="B59" s="0">
+        <v>25.712341197822141</v>
+      </c>
+      <c r="C59" s="0">
+        <v>37.624043715846994</v>
+      </c>
+      <c r="D59" s="0">
+        <v>14.897106109324758</v>
+      </c>
+      <c r="E59" s="0">
+        <v>11.592592592592593</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>41.32096039740582</v>
+      </c>
+      <c r="B60" s="0">
+        <v>30.244101633393829</v>
+      </c>
+      <c r="C60" s="0">
+        <v>43.474681238615666</v>
+      </c>
+      <c r="D60" s="0">
+        <v>18.790996784565916</v>
+      </c>
+      <c r="E60" s="0">
+        <v>14.28888888888889</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>38.907409962743202</v>
+      </c>
+      <c r="B61" s="0">
+        <v>29.719600725952812</v>
+      </c>
+      <c r="C61" s="0">
+        <v>44.60014571948998</v>
+      </c>
+      <c r="D61" s="0">
+        <v>18.418006430868168</v>
+      </c>
+      <c r="E61" s="0">
+        <v>13.503703703703703</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>81.198426935283564</v>
+      </c>
+      <c r="B62" s="0">
+        <v>52.520871143375679</v>
+      </c>
+      <c r="C62" s="0">
+        <v>69.875482695810561</v>
+      </c>
+      <c r="D62" s="0">
+        <v>39.073954983922832</v>
+      </c>
+      <c r="E62" s="0">
+        <v>26.140740740740739</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>59.36014902718366</v>
+      </c>
+      <c r="B63" s="0">
+        <v>45.658802177858441</v>
+      </c>
+      <c r="C63" s="0">
+        <v>63.084153005464479</v>
+      </c>
+      <c r="D63" s="0">
+        <v>34.440514469453376</v>
+      </c>
+      <c r="E63" s="0">
+        <v>24.022222222222222</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>63.476473023319997</v>
+      </c>
+      <c r="B64" s="0">
+        <v>48.014519056261342</v>
+      </c>
+      <c r="C64" s="0">
+        <v>63.926120218579236</v>
+      </c>
+      <c r="D64" s="0">
+        <v>36.749196141479096</v>
+      </c>
+      <c r="E64" s="0">
+        <v>24.829629629629629</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>63.144197599006489</v>
+      </c>
+      <c r="B65" s="0">
+        <v>48.669691470054445</v>
+      </c>
+      <c r="C65" s="0">
+        <v>63.274608378870674</v>
+      </c>
+      <c r="D65" s="0">
+        <v>37.874598070739552</v>
+      </c>
+      <c r="E65" s="0">
+        <v>25.696296296296296</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>77.864495653373808</v>
+      </c>
+      <c r="B66" s="0">
+        <v>55.002722323048999</v>
+      </c>
+      <c r="C66" s="0">
+        <v>73.942222222222227</v>
+      </c>
+      <c r="D66" s="0">
+        <v>43.59163987138264</v>
+      </c>
+      <c r="E66" s="0">
+        <v>30.355555555555554</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>54.673796053539398</v>
+      </c>
+      <c r="B67" s="0">
+        <v>33.032667876588022</v>
+      </c>
+      <c r="C67" s="0">
+        <v>45.019599271402548</v>
+      </c>
+      <c r="D67" s="0">
+        <v>21.173633440514468</v>
+      </c>
+      <c r="E67" s="0">
+        <v>15.207407407407407</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>66.592383055057269</v>
+      </c>
+      <c r="B68" s="0">
+        <v>38.269509981851179</v>
+      </c>
+      <c r="C68" s="0">
+        <v>59.759125683060113</v>
+      </c>
+      <c r="D68" s="0">
+        <v>26.868167202572348</v>
+      </c>
+      <c r="E68" s="0">
+        <v>19.140740740740739</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>65.62315440872085</v>
+      </c>
+      <c r="B69" s="0">
+        <v>39.254990925589837</v>
+      </c>
+      <c r="C69" s="0">
+        <v>65.466958105646626</v>
+      </c>
+      <c r="D69" s="0">
+        <v>28.569131832797428</v>
+      </c>
+      <c r="E69" s="0">
+        <v>20.066666666666666</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>63.54905478128881</v>
+      </c>
+      <c r="B70" s="0">
+        <v>39.153357531760435</v>
+      </c>
+      <c r="C70" s="0">
+        <v>62.941566484517303</v>
+      </c>
+      <c r="D70" s="0">
+        <v>28.289389067524116</v>
+      </c>
+      <c r="E70" s="0">
+        <v>20.022222222222222</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>66.680143507658343</v>
+      </c>
+      <c r="B71" s="0">
+        <v>37.985480943738658</v>
+      </c>
+      <c r="C71" s="0">
+        <v>57.183096539162115</v>
+      </c>
+      <c r="D71" s="0">
+        <v>26.887459807073956</v>
+      </c>
+      <c r="E71" s="0">
+        <v>19.074074074074073</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>57.250862425831379</v>
+      </c>
+      <c r="B72" s="0">
+        <v>29.351179673321234</v>
+      </c>
+      <c r="C72" s="0">
+        <v>60.14448087431694</v>
+      </c>
+      <c r="D72" s="0">
+        <v>15.234726688102894</v>
+      </c>
+      <c r="E72" s="0">
+        <v>12.407407407407407</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0">
+        <v>65.741134262453429</v>
+      </c>
+      <c r="B73" s="0">
+        <v>27.712341197822141</v>
+      </c>
+      <c r="C73" s="0">
+        <v>54.222586520947175</v>
+      </c>
+      <c r="D73" s="0">
+        <v>14.2508038585209</v>
+      </c>
+      <c r="E73" s="0">
+        <v>11.770370370370371</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0">
+        <v>63.485442251966333</v>
+      </c>
+      <c r="B74" s="0">
+        <v>28.078947368421051</v>
+      </c>
+      <c r="C74" s="0">
+        <v>56.139016393442624</v>
+      </c>
+      <c r="D74" s="0">
+        <v>14.90032154340836</v>
+      </c>
+      <c r="E74" s="0">
+        <v>12.481481481481481</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0">
+        <v>61.661929074099625</v>
+      </c>
+      <c r="B75" s="0">
+        <v>27.685117967332122</v>
+      </c>
+      <c r="C75" s="0">
+        <v>50.411001821493628</v>
+      </c>
+      <c r="D75" s="0">
+        <v>14.218649517684888</v>
+      </c>
+      <c r="E75" s="0">
+        <v>12.192592592592593</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0">
+        <v>62.641920794811647</v>
+      </c>
+      <c r="B76" s="0">
+        <v>28.636116152450089</v>
+      </c>
+      <c r="C76" s="0">
+        <v>59.713369763205826</v>
+      </c>
+      <c r="D76" s="0">
+        <v>15.112540192926046</v>
+      </c>
+      <c r="E76" s="0">
+        <v>13.02962962962963</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0">
+        <v>83.674623982337522</v>
+      </c>
+      <c r="B77" s="0">
+        <v>43.379310344827587</v>
+      </c>
+      <c r="C77" s="0">
+        <v>64.662513661202183</v>
+      </c>
+      <c r="D77" s="0">
+        <v>28.488745980707396</v>
+      </c>
+      <c r="E77" s="0">
+        <v>19.992592592592594</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>77.752863253760182</v>
+      </c>
+      <c r="B78" s="0">
+        <v>41.366606170598914</v>
+      </c>
+      <c r="C78" s="0">
+        <v>67.074681238615668</v>
+      </c>
+      <c r="D78" s="0">
+        <v>26.524115755627008</v>
+      </c>
+      <c r="E78" s="0">
+        <v>18.170370370370371</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>70.391748309645365</v>
+      </c>
+      <c r="B79" s="0">
+        <v>46.96551724137931</v>
+      </c>
+      <c r="C79" s="0">
+        <v>72.84072859744991</v>
+      </c>
+      <c r="D79" s="0">
+        <v>30.376205787781352</v>
+      </c>
+      <c r="E79" s="0">
+        <v>20.888888888888889</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>85.171657237477575</v>
+      </c>
+      <c r="B80" s="0">
+        <v>49.503629764065337</v>
+      </c>
+      <c r="C80" s="0">
+        <v>78.629799635701275</v>
+      </c>
+      <c r="D80" s="0">
+        <v>33.212218649517688</v>
+      </c>
+      <c r="E80" s="0">
+        <v>22.74074074074074</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>86.826548916793158</v>
+      </c>
+      <c r="B81" s="0">
+        <v>48.812159709618875</v>
+      </c>
+      <c r="C81" s="0">
+        <v>78.904262295081963</v>
+      </c>
+      <c r="D81" s="0">
+        <v>34.176848874598072</v>
+      </c>
+      <c r="E81" s="0">
+        <v>23.481481481481481</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>70.940665102801162</v>
+      </c>
+      <c r="B82" s="0">
+        <v>34.87295825771325</v>
+      </c>
+      <c r="C82" s="0">
+        <v>61.556284153005464</v>
+      </c>
+      <c r="D82" s="0">
+        <v>20.980707395498392</v>
+      </c>
+      <c r="E82" s="0">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>54.849040982475508</v>
+      </c>
+      <c r="B83" s="0">
+        <v>29.181488203266788</v>
+      </c>
+      <c r="C83" s="0">
+        <v>54.02673952641166</v>
+      </c>
+      <c r="D83" s="0">
+        <v>18.09646302250804</v>
+      </c>
+      <c r="E83" s="0">
+        <v>11.125925925925927</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>75.848075065544364</v>
+      </c>
+      <c r="B84" s="0">
+        <v>33.628856624319418</v>
+      </c>
+      <c r="C84" s="0">
+        <v>58.605755919854282</v>
+      </c>
+      <c r="D84" s="0">
+        <v>20.212218649517684</v>
+      </c>
+      <c r="E84" s="0">
+        <v>12.162962962962963</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>67.16144611563405</v>
+      </c>
+      <c r="B85" s="0">
+        <v>33.466424682395647</v>
+      </c>
+      <c r="C85" s="0">
+        <v>58.859380692167576</v>
+      </c>
+      <c r="D85" s="0">
+        <v>19.356913183279744</v>
+      </c>
+      <c r="E85" s="0">
+        <v>12.548148148148147</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>72.962743204084447</v>
+      </c>
+      <c r="B86" s="0">
+        <v>35.168784029038115</v>
+      </c>
+      <c r="C86" s="0">
+        <v>60.988561020036428</v>
+      </c>
+      <c r="D86" s="0">
+        <v>22.041800643086816</v>
+      </c>
+      <c r="E86" s="0">
+        <v>13.866666666666667</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>63.273216503380709</v>
+      </c>
+      <c r="B87" s="0">
+        <v>35.940108892921963</v>
+      </c>
+      <c r="C87" s="0">
+        <v>62.062513661202189</v>
+      </c>
+      <c r="D87" s="0">
+        <v>28.334405144694532</v>
+      </c>
+      <c r="E87" s="0">
+        <v>23.57037037037037</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>66.91706913205465</v>
+      </c>
+      <c r="B88" s="0">
+        <v>43.115245009074407</v>
+      </c>
+      <c r="C88" s="0">
+        <v>72.754025500910743</v>
+      </c>
+      <c r="D88" s="0">
+        <v>33.79742765273312</v>
+      </c>
+      <c r="E88" s="0">
+        <v>28.414814814814815</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>83.069821995308402</v>
+      </c>
+      <c r="B89" s="0">
+        <v>47.039927404718696</v>
+      </c>
+      <c r="C89" s="0">
+        <v>79.225355191256824</v>
+      </c>
+      <c r="D89" s="0">
+        <v>36.511254019292608</v>
+      </c>
+      <c r="E89" s="0">
+        <v>30.881481481481483</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>86.125431212915686</v>
+      </c>
+      <c r="B90" s="0">
+        <v>52.26678765880218</v>
+      </c>
+      <c r="C90" s="0">
+        <v>80.693624772313299</v>
+      </c>
+      <c r="D90" s="0">
+        <v>38.617363344051448</v>
+      </c>
+      <c r="E90" s="0">
+        <v>33.829629629629629</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0">
+        <v>79.600248378639435</v>
+      </c>
+      <c r="B91" s="0">
+        <v>41.80127041742287</v>
+      </c>
+      <c r="C91" s="0">
+        <v>67.017704918032791</v>
+      </c>
+      <c r="D91" s="0">
+        <v>30.627009646302252</v>
+      </c>
+      <c r="E91" s="0">
+        <v>25.792592592592591</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0">
+        <v>48.145577480336691</v>
+      </c>
+      <c r="B92" s="0">
+        <v>29.54627949183303</v>
+      </c>
+      <c r="C92" s="0">
+        <v>47.528743169398908</v>
+      </c>
+      <c r="D92" s="0">
+        <v>19.212218649517684</v>
+      </c>
+      <c r="E92" s="0">
+        <v>15.785185185185185</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0">
+        <v>54.168483510418106</v>
+      </c>
+      <c r="B93" s="0">
+        <v>32.491833030852995</v>
+      </c>
+      <c r="C93" s="0">
+        <v>51.925027322404368</v>
+      </c>
+      <c r="D93" s="0">
+        <v>20.762057877813504</v>
+      </c>
+      <c r="E93" s="0">
+        <v>17.111111111111111</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0">
+        <v>63.552918449013383</v>
+      </c>
+      <c r="B94" s="0">
+        <v>37.911070780399271</v>
+      </c>
+      <c r="C94" s="0">
+        <v>61.499380692167577</v>
+      </c>
+      <c r="D94" s="0">
+        <v>24.569131832797428</v>
+      </c>
+      <c r="E94" s="0">
+        <v>20.451851851851853</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>58.543673244101008</v>
+      </c>
+      <c r="B95" s="0">
+        <v>35.054446460980039</v>
+      </c>
+      <c r="C95" s="0">
+        <v>55.060546448087429</v>
+      </c>
+      <c r="D95" s="0">
+        <v>22.958199356913184</v>
+      </c>
+      <c r="E95" s="0">
+        <v>18.962962962962962</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>56.486822133296535</v>
+      </c>
+      <c r="B96" s="0">
+        <v>32.726860254083483</v>
+      </c>
+      <c r="C96" s="0">
+        <v>55.254426229508198</v>
+      </c>
+      <c r="D96" s="0">
+        <v>21.620578778135048</v>
+      </c>
+      <c r="E96" s="0">
+        <v>17.644444444444446</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>86.891265351179797</v>
+      </c>
+      <c r="B97" s="0">
+        <v>40.324863883847549</v>
+      </c>
+      <c r="C97" s="0">
+        <v>84.875118397085615</v>
+      </c>
+      <c r="D97" s="0">
+        <v>29.469453376205788</v>
+      </c>
+      <c r="E97" s="0">
+        <v>18.444444444444443</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>70.128604939975162</v>
+      </c>
+      <c r="B98" s="0">
+        <v>30.614337568058076</v>
+      </c>
+      <c r="C98" s="0">
+        <v>63.393078324225868</v>
+      </c>
+      <c r="D98" s="0">
+        <v>21.257234726688104</v>
+      </c>
+      <c r="E98" s="0">
+        <v>13.444444444444445</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>71.608941631019732</v>
+      </c>
+      <c r="B99" s="0">
+        <v>35.866606170598914</v>
+      </c>
+      <c r="C99" s="0">
+        <v>70.792422586520942</v>
+      </c>
+      <c r="D99" s="0">
+        <v>24.655948553054664</v>
+      </c>
+      <c r="E99" s="0">
+        <v>14.962962962962964</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
+        <v>81.745135918311021</v>
+      </c>
+      <c r="B100" s="0">
+        <v>38.917422867513615</v>
+      </c>
+      <c r="C100" s="0">
+        <v>81.78768670309654</v>
+      </c>
+      <c r="D100" s="0">
+        <v>27.69774919614148</v>
+      </c>
+      <c r="E100" s="0">
+        <v>17.511111111111113</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0">
+        <v>80.871809024423897</v>
+      </c>
+      <c r="B101" s="0">
+        <v>36.406533575317603</v>
+      </c>
+      <c r="C101" s="0">
+        <v>69.09100182149362</v>
+      </c>
+      <c r="D101" s="0">
+        <v>25.524115755627008</v>
+      </c>
+      <c r="E101" s="0">
+        <v>15.540740740740741</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0">
+        <v>87.756864909617775</v>
+      </c>
+      <c r="B102" s="0">
+        <v>40.021778584392017</v>
+      </c>
+      <c r="C102" s="0">
+        <v>58.344990892531875</v>
+      </c>
+      <c r="D102" s="0">
+        <v>32.778135048231512</v>
+      </c>
+      <c r="E102" s="0">
+        <v>23.118518518518517</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0">
+        <v>70.824617082930871</v>
+      </c>
+      <c r="B103" s="0">
+        <v>36.023593466424686</v>
+      </c>
+      <c r="C103" s="0">
+        <v>58.204371584699452</v>
+      </c>
+      <c r="D103" s="0">
+        <v>31.385852090032156</v>
+      </c>
+      <c r="E103" s="0">
+        <v>22.451851851851853</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0">
+        <v>74.692010487098116</v>
+      </c>
+      <c r="B104" s="0">
+        <v>37.080762250453724</v>
+      </c>
+      <c r="C104" s="0">
+        <v>62.648233151183973</v>
+      </c>
+      <c r="D104" s="0">
+        <v>32.659163987138264</v>
+      </c>
+      <c r="E104" s="0">
+        <v>22.081481481481482</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0">
+        <v>76.092866013522837</v>
+      </c>
+      <c r="B105" s="0">
+        <v>40.848457350272234</v>
+      </c>
+      <c r="C105" s="0">
+        <v>59.66098360655738</v>
+      </c>
+      <c r="D105" s="0">
+        <v>33.186495176848872</v>
+      </c>
+      <c r="E105" s="0">
+        <v>23.977777777777778</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0">
+        <v>84.465295984545335</v>
+      </c>
+      <c r="B106" s="0">
+        <v>39.783121597096191</v>
+      </c>
+      <c r="C106" s="0">
+        <v>59.724954462659383</v>
+      </c>
+      <c r="D106" s="0">
+        <v>34.347266881028936</v>
+      </c>
+      <c r="E106" s="0">
+        <v>24.666666666666668</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0">
+        <v>52.276114254174139</v>
+      </c>
+      <c r="B107" s="0">
+        <v>28.991833030852995</v>
+      </c>
+      <c r="C107" s="0">
+        <v>44.084954462659383</v>
+      </c>
+      <c r="D107" s="0">
+        <v>22.627009646302252</v>
+      </c>
+      <c r="E107" s="0">
+        <v>19.25925925925926</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0">
+        <v>67.809714364564641</v>
+      </c>
+      <c r="B108" s="0">
+        <v>33.408348457350272</v>
+      </c>
+      <c r="C108" s="0">
+        <v>55.789945355191257</v>
+      </c>
+      <c r="D108" s="0">
+        <v>25.980707395498392</v>
+      </c>
+      <c r="E108" s="0">
+        <v>22.029629629629628</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0">
+        <v>72.876086656547542</v>
+      </c>
+      <c r="B109" s="0">
+        <v>37.770417422867517</v>
+      </c>
+      <c r="C109" s="0">
+        <v>56.432276867030964</v>
+      </c>
+      <c r="D109" s="0">
+        <v>31.70418006430868</v>
+      </c>
+      <c r="E109" s="0">
+        <v>25.785185185185185</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0">
+        <v>64.081412998482136</v>
+      </c>
+      <c r="B110" s="0">
+        <v>37.627949183303087</v>
+      </c>
+      <c r="C110" s="0">
+        <v>58.081967213114751</v>
+      </c>
+      <c r="D110" s="0">
+        <v>29.176848874598072</v>
+      </c>
+      <c r="E110" s="0">
+        <v>24.362962962962964</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0">
+        <v>70.413964399061683</v>
+      </c>
+      <c r="B111" s="0">
+        <v>38.780399274047184</v>
+      </c>
+      <c r="C111" s="0">
+        <v>54.642987249544625</v>
+      </c>
+      <c r="D111" s="0">
+        <v>30.372990353697748</v>
+      </c>
+      <c r="E111" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0">
+        <v>73.108320684421145</v>
+      </c>
+      <c r="B112" s="0">
+        <v>39.427404718693282</v>
+      </c>
+      <c r="C112" s="0">
+        <v>56.792349726775953</v>
+      </c>
+      <c r="D112" s="0">
+        <v>23.424437299035368</v>
+      </c>
+      <c r="E112" s="0">
+        <v>15.585185185185185</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0">
+        <v>52.633641506830415</v>
+      </c>
+      <c r="B113" s="0">
+        <v>34.14246823956443</v>
+      </c>
+      <c r="C113" s="0">
+        <v>55.683424408014574</v>
+      </c>
+      <c r="D113" s="0">
+        <v>21.15434083601286</v>
+      </c>
+      <c r="E113" s="0">
+        <v>14.281481481481482</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0">
+        <v>61.671036290878988</v>
+      </c>
+      <c r="B114" s="0">
+        <v>38.820326678765881</v>
+      </c>
+      <c r="C114" s="0">
+        <v>59.682112932604738</v>
+      </c>
+      <c r="D114" s="0">
+        <v>23.138263665594856</v>
+      </c>
+      <c r="E114" s="0">
+        <v>15.637037037037038</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0">
+        <v>62.024975852076722</v>
+      </c>
+      <c r="B115" s="0">
+        <v>39.722323049001815</v>
+      </c>
+      <c r="C115" s="0">
+        <v>54.748779599271401</v>
+      </c>
+      <c r="D115" s="0">
+        <v>23.79742765273312</v>
+      </c>
+      <c r="E115" s="0">
+        <v>15.562962962962963</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0">
+        <v>70.655857596246719</v>
+      </c>
+      <c r="B116" s="0">
+        <v>41.302177858439201</v>
+      </c>
+      <c r="C116" s="0">
+        <v>61.94222222222222</v>
+      </c>
+      <c r="D116" s="0">
+        <v>24.874598070739548</v>
+      </c>
+      <c r="E116" s="0">
+        <v>16.103703703703705</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0">
+        <v>50.919276942182975</v>
+      </c>
+      <c r="B117" s="0">
+        <v>33.782214156079853</v>
+      </c>
+      <c r="C117" s="0">
+        <v>53.672786885245898</v>
+      </c>
+      <c r="D117" s="0">
+        <v>29.713826366559484</v>
+      </c>
+      <c r="E117" s="0">
+        <v>20.355555555555554</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0">
+        <v>59.166551676555819</v>
+      </c>
+      <c r="B118" s="0">
+        <v>36.647005444646098</v>
+      </c>
+      <c r="C118" s="0">
+        <v>66.575664845173037</v>
+      </c>
+      <c r="D118" s="0">
+        <v>34.784565916398712</v>
+      </c>
+      <c r="E118" s="0">
+        <v>23.918518518518518</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0">
+        <v>65.46888367600387</v>
+      </c>
+      <c r="B119" s="0">
+        <v>36.068965517241381</v>
+      </c>
+      <c r="C119" s="0">
+        <v>63.153806921675773</v>
+      </c>
+      <c r="D119" s="0">
+        <v>32.726688102893888</v>
+      </c>
+      <c r="E119" s="0">
+        <v>21.962962962962962</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0">
+        <v>58.831378501448874</v>
+      </c>
+      <c r="B120" s="0">
+        <v>37.918330308529946</v>
+      </c>
+      <c r="C120" s="0">
+        <v>62.873734061930783</v>
+      </c>
+      <c r="D120" s="0">
+        <v>37.276527331189712</v>
+      </c>
+      <c r="E120" s="0">
+        <v>25.962962962962962</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0">
+        <v>64.878156478542849</v>
+      </c>
+      <c r="B121" s="0">
+        <v>37.402903811252266</v>
+      </c>
+      <c r="C121" s="0">
+        <v>62.730200364298724</v>
+      </c>
+      <c r="D121" s="0">
+        <v>36.572347266881032</v>
+      </c>
+      <c r="E121" s="0">
+        <v>24.881481481481483</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0">
+        <v>73.189319718504208</v>
+      </c>
+      <c r="B122" s="0">
+        <v>44.867513611615244</v>
+      </c>
+      <c r="C122" s="0">
+        <v>70.981639344262291</v>
+      </c>
+      <c r="D122" s="0">
+        <v>37.768488745980704</v>
+      </c>
+      <c r="E122" s="0">
+        <v>31.392592592592592</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0">
+        <v>56.548778805022771</v>
+      </c>
+      <c r="B123" s="0">
+        <v>33.668784029038115</v>
+      </c>
+      <c r="C123" s="0">
+        <v>50.312276867030967</v>
+      </c>
+      <c r="D123" s="0">
+        <v>27.639871382636656</v>
+      </c>
+      <c r="E123" s="0">
+        <v>23.414814814814815</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0">
+        <v>72.87663860907962</v>
+      </c>
+      <c r="B124" s="0">
+        <v>42.736842105263158</v>
+      </c>
+      <c r="C124" s="0">
+        <v>63.72990892531876</v>
+      </c>
+      <c r="D124" s="0">
+        <v>37.80385852090032</v>
+      </c>
+      <c r="E124" s="0">
+        <v>31.214814814814815</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0">
+        <v>73.397819787498278</v>
+      </c>
+      <c r="B125" s="0">
+        <v>45.42831215970962</v>
+      </c>
+      <c r="C125" s="0">
+        <v>73.4576320582878</v>
+      </c>
+      <c r="D125" s="0">
+        <v>39.60450160771704</v>
+      </c>
+      <c r="E125" s="0">
+        <v>32.585185185185182</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0">
+        <v>73.892921208776045</v>
+      </c>
+      <c r="B126" s="0">
+        <v>46.556261343012707</v>
+      </c>
+      <c r="C126" s="0">
+        <v>70.897996357012744</v>
+      </c>
+      <c r="D126" s="0">
+        <v>38.353697749196144</v>
+      </c>
+      <c r="E126" s="0">
+        <v>32.37777777777778</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0">
+        <v>44.469849592935006</v>
+      </c>
+      <c r="B127" s="0">
+        <v>29.725045372050818</v>
+      </c>
+      <c r="C127" s="0">
+        <v>37.678469945355189</v>
+      </c>
+      <c r="D127" s="0">
+        <v>23.19614147909968</v>
+      </c>
+      <c r="E127" s="0">
+        <v>14.34074074074074</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0">
+        <v>55.597764592245063</v>
+      </c>
+      <c r="B128" s="0">
+        <v>32.37295825771325</v>
+      </c>
+      <c r="C128" s="0">
+        <v>43.68109289617486</v>
+      </c>
+      <c r="D128" s="0">
+        <v>26.819935691318328</v>
+      </c>
+      <c r="E128" s="0">
+        <v>15.533333333333333</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0">
+        <v>42.700013798813302</v>
+      </c>
+      <c r="B129" s="0">
+        <v>27.879310344827587</v>
+      </c>
+      <c r="C129" s="0">
+        <v>36.147030965391622</v>
+      </c>
+      <c r="D129" s="0">
+        <v>23.488745980707396</v>
+      </c>
+      <c r="E129" s="0">
+        <v>13.303703703703704</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0">
+        <v>49.099351455774801</v>
+      </c>
+      <c r="B130" s="0">
+        <v>30.249546279491835</v>
+      </c>
+      <c r="C130" s="0">
+        <v>38.24335154826958</v>
+      </c>
+      <c r="D130" s="0">
+        <v>26.69774919614148</v>
+      </c>
+      <c r="E130" s="0">
+        <v>15.725925925925926</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0">
+        <v>43.486684145163515</v>
+      </c>
+      <c r="B131" s="0">
+        <v>27.099818511796734</v>
+      </c>
+      <c r="C131" s="0">
+        <v>37.060255009107465</v>
+      </c>
+      <c r="D131" s="0">
+        <v>23.321543408360128</v>
+      </c>
+      <c r="E131" s="0">
+        <v>14.118518518518519</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0">
+        <v>63.328549744721954</v>
+      </c>
+      <c r="B132" s="0">
+        <v>50.148820326678766</v>
+      </c>
+      <c r="C132" s="0">
+        <v>65.246848816029143</v>
+      </c>
+      <c r="D132" s="0">
+        <v>37.028938906752408</v>
+      </c>
+      <c r="E132" s="0">
+        <v>39.540740740740738</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0">
+        <v>70.095625776183255</v>
+      </c>
+      <c r="B133" s="0">
+        <v>48.081669691470054</v>
+      </c>
+      <c r="C133" s="0">
+        <v>64.029508196721309</v>
+      </c>
+      <c r="D133" s="0">
+        <v>34.9967845659164</v>
+      </c>
+      <c r="E133" s="0">
+        <v>36.970370370370368</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0">
+        <v>70.892921208776045</v>
+      </c>
+      <c r="B134" s="0">
+        <v>46.160617059891109</v>
+      </c>
+      <c r="C134" s="0">
+        <v>59.956284153005463</v>
+      </c>
+      <c r="D134" s="0">
+        <v>31.469453376205788</v>
+      </c>
+      <c r="E134" s="0">
+        <v>34.511111111111113</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0">
+        <v>68.574858562163655</v>
+      </c>
+      <c r="B135" s="0">
+        <v>45.901088929219604</v>
+      </c>
+      <c r="C135" s="0">
+        <v>57.161311475409839</v>
+      </c>
+      <c r="D135" s="0">
+        <v>31.5048231511254</v>
+      </c>
+      <c r="E135" s="0">
+        <v>33.548148148148151</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0">
+        <v>71.418242031185315</v>
+      </c>
+      <c r="B136" s="0">
+        <v>44.890199637023592</v>
+      </c>
+      <c r="C136" s="0">
+        <v>58.937559198542807</v>
+      </c>
+      <c r="D136" s="0">
+        <v>31.421221864951768</v>
+      </c>
+      <c r="E136" s="0">
+        <v>33.88148148148148</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0">
+        <v>75.436456464744026</v>
+      </c>
+      <c r="B137" s="0">
+        <v>34.382032667876587</v>
+      </c>
+      <c r="C137" s="0">
+        <v>58.21814207650273</v>
+      </c>
+      <c r="D137" s="0">
+        <v>14.572347266881028</v>
+      </c>
+      <c r="E137" s="0">
+        <v>11.837037037037037</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0">
+        <v>66.334897198840906</v>
+      </c>
+      <c r="B138" s="0">
+        <v>31.701451905626133</v>
+      </c>
+      <c r="C138" s="0">
+        <v>54.684080145719491</v>
+      </c>
+      <c r="D138" s="0">
+        <v>12.70096463022508</v>
+      </c>
+      <c r="E138" s="0">
+        <v>10.540740740740741</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0">
+        <v>74.430384986891127</v>
+      </c>
+      <c r="B139" s="0">
+        <v>38.539019963702358</v>
+      </c>
+      <c r="C139" s="0">
+        <v>63.053260473588345</v>
+      </c>
+      <c r="D139" s="0">
+        <v>17.122186495176848</v>
+      </c>
+      <c r="E139" s="0">
+        <v>13.97037037037037</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0">
+        <v>72.650062094659859</v>
+      </c>
+      <c r="B140" s="0">
+        <v>39.92558983666062</v>
+      </c>
+      <c r="C140" s="0">
+        <v>62.504262295081965</v>
+      </c>
+      <c r="D140" s="0">
+        <v>18.491961414790996</v>
+      </c>
+      <c r="E140" s="0">
+        <v>15.474074074074075</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0">
+        <v>61.900372567959153</v>
+      </c>
+      <c r="B141" s="0">
+        <v>35.597096188747734</v>
+      </c>
+      <c r="C141" s="0">
+        <v>55.729180327868853</v>
+      </c>
+      <c r="D141" s="0">
+        <v>15.694533762057878</v>
+      </c>
+      <c r="E141" s="0">
+        <v>13.103703703703705</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0">
+        <v>92.579136194287287</v>
+      </c>
+      <c r="B142" s="0">
+        <v>43.78856624319419</v>
+      </c>
+      <c r="C142" s="0">
+        <v>65.546666666666667</v>
+      </c>
+      <c r="D142" s="0">
+        <v>26.7491961414791</v>
+      </c>
+      <c r="E142" s="0">
+        <v>21.392592592592592</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0">
+        <v>68.413964399061683</v>
+      </c>
+      <c r="B143" s="0">
+        <v>36.242286751361164</v>
+      </c>
+      <c r="C143" s="0">
+        <v>53.814207650273225</v>
+      </c>
+      <c r="D143" s="0">
+        <v>22.205787781350484</v>
+      </c>
+      <c r="E143" s="0">
+        <v>17.096296296296295</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0">
+        <v>75.934593624948249</v>
+      </c>
+      <c r="B144" s="0">
+        <v>43.565335753176043</v>
+      </c>
+      <c r="C144" s="0">
+        <v>65.727140255009104</v>
+      </c>
+      <c r="D144" s="0">
+        <v>29.086816720257236</v>
+      </c>
+      <c r="E144" s="0">
+        <v>23.68888888888889</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0">
+        <v>75.531530288395203</v>
+      </c>
+      <c r="B145" s="0">
+        <v>40.989110707803995</v>
+      </c>
+      <c r="C145" s="0">
+        <v>63.136029143897993</v>
+      </c>
+      <c r="D145" s="0">
+        <v>25.768488745980708</v>
+      </c>
+      <c r="E145" s="0">
+        <v>20.644444444444446</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0">
+        <v>75.438526286739346</v>
+      </c>
+      <c r="B146" s="0">
+        <v>44.350272232304903</v>
+      </c>
+      <c r="C146" s="0">
+        <v>71.135737704918029</v>
+      </c>
+      <c r="D146" s="0">
+        <v>28.95176848874598</v>
+      </c>
+      <c r="E146" s="0">
+        <v>23.422222222222221</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0">
+        <v>89.730233199944806</v>
+      </c>
+      <c r="B147" s="0">
+        <v>53.996370235934663</v>
+      </c>
+      <c r="C147" s="0">
+        <v>93.081530054644816</v>
+      </c>
+      <c r="D147" s="0">
+        <v>43.10932475884244</v>
+      </c>
+      <c r="E147" s="0">
+        <v>37.214814814814815</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0">
+        <v>77.670760314612949</v>
+      </c>
+      <c r="B148" s="0">
+        <v>47.822141560798549</v>
+      </c>
+      <c r="C148" s="0">
+        <v>76.679052823315118</v>
+      </c>
+      <c r="D148" s="0">
+        <v>36.39871382636656</v>
+      </c>
+      <c r="E148" s="0">
+        <v>31.585185185185185</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0">
+        <v>83.238029529460462</v>
+      </c>
+      <c r="B149" s="0">
+        <v>50.238656987295826</v>
+      </c>
+      <c r="C149" s="0">
+        <v>90.697340619307838</v>
+      </c>
+      <c r="D149" s="0">
+        <v>38.318327974276528</v>
+      </c>
+      <c r="E149" s="0">
+        <v>32.422222222222224</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0">
+        <v>92.717538291706916</v>
+      </c>
+      <c r="B150" s="0">
+        <v>53.536297640653359</v>
+      </c>
+      <c r="C150" s="0">
+        <v>94.800510018214936</v>
+      </c>
+      <c r="D150" s="0">
+        <v>42.372990353697752</v>
+      </c>
+      <c r="E150" s="0">
+        <v>36.103703703703701</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0">
+        <v>92.142403753277222</v>
+      </c>
+      <c r="B151" s="0">
+        <v>52.964609800362979</v>
+      </c>
+      <c r="C151" s="0">
+        <v>92.223752276867032</v>
+      </c>
+      <c r="D151" s="0">
+        <v>41.453376205787784</v>
+      </c>
+      <c r="E151" s="0">
+        <v>35.451851851851849</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0">
+        <v>70.945494687456872</v>
+      </c>
+      <c r="B152" s="0">
+        <v>43.10526315789474</v>
+      </c>
+      <c r="C152" s="0">
+        <v>69.599562841530059</v>
+      </c>
+      <c r="D152" s="0">
+        <v>34.836012861736336</v>
+      </c>
+      <c r="E152" s="0">
+        <v>27.770370370370369</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0">
+        <v>54.50986615151097</v>
+      </c>
+      <c r="B153" s="0">
+        <v>33.069872958257712</v>
+      </c>
+      <c r="C153" s="0">
+        <v>54.132167577413476</v>
+      </c>
+      <c r="D153" s="0">
+        <v>29.662379421221864</v>
+      </c>
+      <c r="E153" s="0">
+        <v>21.748148148148147</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0">
+        <v>61.769697805988685</v>
+      </c>
+      <c r="B154" s="0">
+        <v>37.568965517241381</v>
+      </c>
+      <c r="C154" s="0">
+        <v>60.366630236794173</v>
+      </c>
+      <c r="D154" s="0">
+        <v>32.69774919614148</v>
+      </c>
+      <c r="E154" s="0">
+        <v>24.029629629629628</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0">
+        <v>62.811370222160896</v>
+      </c>
+      <c r="B155" s="0">
+        <v>41.866606170598914</v>
+      </c>
+      <c r="C155" s="0">
+        <v>58.642112932604739</v>
+      </c>
+      <c r="D155" s="0">
+        <v>34.450160771704184</v>
+      </c>
+      <c r="E155" s="0">
+        <v>26.977777777777778</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0"/>
+      <c r="B156" s="0"/>
+      <c r="C156" s="0"/>
+      <c r="D156" s="0"/>
+      <c r="E156" s="0"/>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>